<commit_message>
Left Tasks implementing CL and OTM and all PuLP
</commit_message>
<xml_diff>
--- a/Santanu/21 March/Dashboard_Input.xlsx
+++ b/Santanu/21 March/Dashboard_Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Upwork me as ORS\OWFCR\Santanu\21 March\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C7EC70-2B70-4E61-ADEB-6D2A24A190FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A505781-7065-48EB-AE0E-7225B183E3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,6 +148,27 @@
     <t>T25</t>
   </si>
   <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Responde</t>
+  </si>
+  <si>
+    <t>OWFCR-SS</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Maximum number of cables allowed to be connected to each substation</t>
+  </si>
+  <si>
+    <t>1 means consider String Structure and 0 means don’t</t>
+  </si>
+  <si>
     <t>T26</t>
   </si>
   <si>
@@ -221,34 +242,13 @@
   </si>
   <si>
     <t>T50</t>
-  </si>
-  <si>
-    <t>Query</t>
-  </si>
-  <si>
-    <t>Responde</t>
-  </si>
-  <si>
-    <t>OWFCR-SS</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Maximum number of cables allowed to be connected to each substation</t>
-  </si>
-  <si>
-    <t>1 means consider String Structure and 0 means don’t</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +266,36 @@
       <sz val="14"/>
       <name val="Georgia"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -288,15 +318,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,43 +625,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="60.44140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="40.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.44140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>67</v>
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>69</v>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>70</v>
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -634,32 +674,30 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="23.6640625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="4" width="11" customWidth="1"/>
+    <col min="1" max="16384" width="23.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
@@ -668,12 +706,12 @@
       <c r="C2" s="3">
         <v>16.120688940000001</v>
       </c>
-      <c r="D2" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D2" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
@@ -682,12 +720,12 @@
       <c r="C3" s="3">
         <v>14.31034848</v>
       </c>
-      <c r="D3" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D3" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3">
@@ -696,12 +734,12 @@
       <c r="C4" s="3">
         <v>12.844828970000002</v>
       </c>
-      <c r="D4" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D4" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
@@ -710,12 +748,12 @@
       <c r="C5" s="3">
         <v>10.431037420000001</v>
       </c>
-      <c r="D5" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D5" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
@@ -724,12 +762,12 @@
       <c r="C6" s="3">
         <v>8.1896595439999995</v>
       </c>
-      <c r="D6" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="D6" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3">
@@ -738,12 +776,12 @@
       <c r="C7" s="3">
         <v>6.2068989869999998</v>
       </c>
-      <c r="D7" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="D7" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3">
@@ -752,12 +790,12 @@
       <c r="C8" s="3">
         <v>4.5689657940000004</v>
       </c>
-      <c r="D8" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="D8" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="3">
@@ -766,12 +804,12 @@
       <c r="C9" s="3">
         <v>26.551719930000001</v>
       </c>
-      <c r="D9" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="D9" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="3">
@@ -780,12 +818,12 @@
       <c r="C10" s="3">
         <v>21.896556930000003</v>
       </c>
-      <c r="D10" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="D10" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="3">
@@ -794,12 +832,12 @@
       <c r="C11" s="3">
         <v>5.0862068410000001</v>
       </c>
-      <c r="D11" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D11" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="3">
@@ -808,12 +846,12 @@
       <c r="C12" s="3">
         <v>2.5862116559999997</v>
       </c>
-      <c r="D12" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D12" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="3">
@@ -822,12 +860,12 @@
       <c r="C13" s="3">
         <v>0.43103741569999998</v>
       </c>
-      <c r="D13" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D13" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3">
@@ -836,12 +874,12 @@
       <c r="C14" s="3">
         <v>-1.465513091</v>
       </c>
-      <c r="D14" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D14" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="3">
@@ -850,12 +888,12 @@
       <c r="C15" s="3">
         <v>-2.9310326010000001</v>
       </c>
-      <c r="D15" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D15" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="3">
@@ -864,12 +902,12 @@
       <c r="C16" s="3">
         <v>-3.8793046450000004</v>
       </c>
-      <c r="D16" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D16" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="3">
@@ -878,12 +916,12 @@
       <c r="C17" s="3">
         <v>-4.3965456920000001</v>
       </c>
-      <c r="D17" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D17" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="3">
@@ -892,12 +930,12 @@
       <c r="C18" s="3">
         <v>-1.2930994089999999</v>
       </c>
-      <c r="D18" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="D18" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="3">
@@ -906,12 +944,12 @@
       <c r="C19" s="3">
         <v>-3.0172362329999998</v>
       </c>
-      <c r="D19" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D19" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="3">
@@ -920,12 +958,12 @@
       <c r="C20" s="3">
         <v>-26.379306249999999</v>
       </c>
-      <c r="D20" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="D20" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="3">
@@ -934,12 +972,12 @@
       <c r="C21" s="3">
         <v>-2.7586189189999999</v>
       </c>
-      <c r="D21" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="D21" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="3">
@@ -948,12 +986,12 @@
       <c r="C22" s="3">
         <v>-5.2586205240000004</v>
       </c>
-      <c r="D22" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="D22" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="3">
@@ -962,12 +1000,12 @@
       <c r="C23" s="3">
         <v>-7.4137883439999994</v>
       </c>
-      <c r="D23" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="D23" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="3">
@@ -976,12 +1014,12 @@
       <c r="C24" s="3">
         <v>-9.224135218999999</v>
       </c>
-      <c r="D24" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="D24" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="3">
@@ -990,12 +1028,12 @@
       <c r="C25" s="3">
         <v>-10.775858359999999</v>
       </c>
-      <c r="D25" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="D25" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="3">
@@ -1004,13 +1042,13 @@
       <c r="C26" s="3">
         <v>-11.55172314</v>
       </c>
-      <c r="D26" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>39</v>
+      <c r="D26" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B27" s="3">
         <v>3.0399990950000002</v>
@@ -1018,13 +1056,13 @@
       <c r="C27" s="3">
         <v>-11.46551309</v>
       </c>
-      <c r="D27" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>40</v>
+      <c r="D27" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B28" s="3">
         <v>9.1200002619999996</v>
@@ -1032,13 +1070,13 @@
       <c r="C28" s="3">
         <v>-11.63792677</v>
       </c>
-      <c r="D28" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>41</v>
+      <c r="D28" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B29" s="3">
         <v>16.000002680000001</v>
@@ -1046,13 +1084,13 @@
       <c r="C29" s="3">
         <v>-11.37930946</v>
       </c>
-      <c r="D29" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>42</v>
+      <c r="D29" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B30" s="3">
         <v>22.640005169999998</v>
@@ -1060,13 +1098,13 @@
       <c r="C30" s="3">
         <v>-11.724136820000002</v>
       </c>
-      <c r="D30" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>43</v>
+      <c r="D30" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B31" s="3">
         <v>29.200006199999997</v>
@@ -1074,13 +1112,13 @@
       <c r="C31" s="3">
         <v>-11.37930946</v>
       </c>
-      <c r="D31" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>44</v>
+      <c r="D31" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B32" s="3">
         <v>-10.56000281</v>
@@ -1088,13 +1126,13 @@
       <c r="C32" s="3">
         <v>-18.017239440000001</v>
       </c>
-      <c r="D32" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>45</v>
+      <c r="D32" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B33" s="3">
         <v>-5.2800043839999997</v>
@@ -1102,13 +1140,13 @@
       <c r="C33" s="3">
         <v>-19.137925170000003</v>
       </c>
-      <c r="D33" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>46</v>
+      <c r="D33" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B34" s="3">
         <v>0.55999983320000002</v>
@@ -1116,13 +1154,13 @@
       <c r="C34" s="3">
         <v>-19.999993580000002</v>
       </c>
-      <c r="D34" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>47</v>
+      <c r="D34" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B35" s="3">
         <v>6.2400011199999996</v>
@@ -1130,13 +1168,13 @@
       <c r="C35" s="3">
         <v>-20.431031000000001</v>
       </c>
-      <c r="D35" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>48</v>
+      <c r="D35" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B36" s="3">
         <v>11.520002529999999</v>
@@ -1144,13 +1182,13 @@
       <c r="C36" s="3">
         <v>-20.517234629999997</v>
       </c>
-      <c r="D36" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>49</v>
+      <c r="D36" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B37" s="3">
         <v>17.520003719999998</v>
@@ -1158,13 +1196,13 @@
       <c r="C37" s="3">
         <v>-20.517234629999997</v>
       </c>
-      <c r="D37" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>50</v>
+      <c r="D37" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B38" s="3">
         <v>23.120005030000002</v>
@@ -1172,13 +1210,13 @@
       <c r="C38" s="3">
         <v>-19.74137627</v>
       </c>
-      <c r="D38" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>51</v>
+      <c r="D38" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B39" s="3">
         <v>28.560006389999998</v>
@@ -1186,13 +1224,13 @@
       <c r="C39" s="3">
         <v>-18.87930785</v>
       </c>
-      <c r="D39" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>52</v>
+      <c r="D39" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A40" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B40" s="3">
         <v>-4.000004766</v>
@@ -1200,13 +1238,13 @@
       <c r="C40" s="3">
         <v>-27.32758471</v>
       </c>
-      <c r="D40" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>53</v>
+      <c r="D40" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="B41" s="3">
         <v>1.439999571</v>
@@ -1214,13 +1252,13 @@
       <c r="C41" s="3">
         <v>-28.103443069999997</v>
       </c>
-      <c r="D41" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>54</v>
+      <c r="D41" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="B42" s="3">
         <v>7.5200007389999994</v>
@@ -1228,13 +1266,13 @@
       <c r="C42" s="3">
         <v>-28.27585676</v>
       </c>
-      <c r="D42" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>55</v>
+      <c r="D42" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B43" s="3">
         <v>13.04000207</v>
@@ -1242,13 +1280,13 @@
       <c r="C43" s="3">
         <v>-27.931029389999999</v>
       </c>
-      <c r="D43" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>56</v>
+      <c r="D43" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A44" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B44" s="3">
         <v>18.72000336</v>
@@ -1256,13 +1294,13 @@
       <c r="C44" s="3">
         <v>-27.586202029999999</v>
       </c>
-      <c r="D44" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>57</v>
+      <c r="D44" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A45" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B45" s="3">
         <v>24.320006159999998</v>
@@ -1270,13 +1308,13 @@
       <c r="C45" s="3">
         <v>-26.724133609999999</v>
       </c>
-      <c r="D45" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>58</v>
+      <c r="D45" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B46" s="3">
         <v>0.63999980940000001</v>
@@ -1284,13 +1322,13 @@
       <c r="C46" s="3">
         <v>-36.982754140000004</v>
       </c>
-      <c r="D46" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>59</v>
+      <c r="D46" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B47" s="3">
         <v>6.6400010010000008</v>
@@ -1298,13 +1336,13 @@
       <c r="C47" s="3">
         <v>-37.06896098</v>
       </c>
-      <c r="D47" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>60</v>
+      <c r="D47" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B48" s="3">
         <v>12.080002360000002</v>
@@ -1312,13 +1350,13 @@
       <c r="C48" s="3">
         <v>-36.465513090000002</v>
       </c>
-      <c r="D48" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>61</v>
+      <c r="D48" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A49" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="B49" s="3">
         <v>17.440003739999998</v>
@@ -1326,13 +1364,13 @@
       <c r="C49" s="3">
         <v>-36.206892570000001</v>
       </c>
-      <c r="D49" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>62</v>
+      <c r="D49" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B50" s="3">
         <v>23.280004979999998</v>
@@ -1340,13 +1378,13 @@
       <c r="C50" s="3">
         <v>-35.51723784</v>
       </c>
-      <c r="D50" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>63</v>
+      <c r="D50" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A51" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B51" s="3">
         <v>-5.6</v>
@@ -1354,7 +1392,7 @@
       <c r="C51" s="3">
         <v>19.69827445</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="4">
         <v>8</v>
       </c>
     </row>
@@ -1369,71 +1407,71 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="1" max="16384" width="21.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1445,71 +1483,71 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="23.44140625" defaultRowHeight="19.8" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="1" max="16384" width="23.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="8">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="8">
         <v>10</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1521,84 +1559,82 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="27.44140625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="4" width="11" customWidth="1"/>
+    <col min="1" max="16384" width="27.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>24</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>393</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <f>4*8</f>
         <v>32</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>460</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <f>5*8</f>
         <v>40</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>540</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>